<commit_message>
new combined QTL model
</commit_message>
<xml_diff>
--- a/Supplementary_file_QTLsummary_20230309.xlsx
+++ b/Supplementary_file_QTLsummary_20230309.xlsx
@@ -5,20 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wendy/Desktop/manuscript-QTL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wendy/Documents/QTL_manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0BDA73E-A2E5-2C48-8630-758489A4A219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E83760-281C-FE41-9A88-D19F268AE4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7580" yWindow="2480" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{6C94EA74-2405-CA42-B48B-4E9AF06CE556}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23440" windowHeight="14560" activeTab="4" xr2:uid="{6C94EA74-2405-CA42-B48B-4E9AF06CE556}"/>
   </bookViews>
   <sheets>
     <sheet name="deltoides_uni" sheetId="1" r:id="rId1"/>
     <sheet name="nigra_uni" sheetId="4" r:id="rId2"/>
     <sheet name="dosage_uni" sheetId="7" r:id="rId3"/>
-    <sheet name="deltoides_multi" sheetId="10" r:id="rId4"/>
-    <sheet name="nigra_multi" sheetId="14" r:id="rId5"/>
-    <sheet name="dosage_multi" sheetId="15" r:id="rId6"/>
+    <sheet name="Geno3_interactions" sheetId="10" r:id="rId4"/>
+    <sheet name="Geno3_states" sheetId="14" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="373">
   <si>
     <t>Pheno</t>
   </si>
@@ -1105,102 +1104,77 @@
     <t>time_serie_vol</t>
   </si>
   <si>
-    <t>Chr06_13050941_13743520</t>
-  </si>
-  <si>
-    <t>Chr10_14250037_14642137</t>
-  </si>
-  <si>
-    <t>Chr16_6717622_9756840</t>
-  </si>
-  <si>
-    <t>Chr16_12792247_13806265</t>
-  </si>
-  <si>
-    <t>Chr11_1_5087791</t>
-  </si>
-  <si>
-    <t>Chr03_14432880_14602490</t>
-  </si>
-  <si>
-    <t>Chr01_32539630_33198436</t>
-  </si>
-  <si>
-    <t>Chr17_9187852_10189238</t>
-  </si>
-  <si>
-    <t>Chr06_23302831_23932611</t>
-  </si>
-  <si>
-    <t>Chr04_1_2320306</t>
-  </si>
-  <si>
-    <t>Chr04_2791762_3125954</t>
-  </si>
-  <si>
-    <t>Horiz_size_50perc_field_y1_y2</t>
-  </si>
-  <si>
-    <t>Chr04_1_1121053</t>
-  </si>
-  <si>
-    <t>Chr04_1_4548633</t>
-  </si>
-  <si>
-    <t>Chr04_1121054_2320306</t>
-  </si>
-  <si>
-    <t>Chr17_5386482_10189238</t>
-  </si>
-  <si>
-    <t>Chr17_11013136_11823436</t>
-  </si>
-  <si>
-    <t>Chr17_5386482_8218065</t>
-  </si>
-  <si>
-    <t>Chr17_11013136_13646486</t>
-  </si>
-  <si>
-    <t>Chr08_2438318_2661619</t>
-  </si>
-  <si>
-    <t>Chr08_2438318_3724915</t>
-  </si>
-  <si>
-    <t>Chr08_404934_1134976</t>
-  </si>
-  <si>
-    <t>Chr08_1917318_2661619</t>
-  </si>
-  <si>
-    <t>Chr08_3508389_6668474</t>
-  </si>
-  <si>
-    <t>Chr08_8764526_14623837</t>
-  </si>
-  <si>
-    <t>Chr08_4438715_4736958</t>
-  </si>
-  <si>
-    <t>Chr08_9514392_9939820</t>
-  </si>
-  <si>
-    <t>Chr08_10571450_10869433</t>
-  </si>
-  <si>
-    <t>Chr08_3508389_3724915</t>
-  </si>
-  <si>
-    <t>Chr08_1917318_3724915</t>
+    <t>Chr01_27147399_27349178</t>
+  </si>
+  <si>
+    <t>Chr01_29345990_38029566</t>
+  </si>
+  <si>
+    <t>Chr14_12576375_13044173</t>
+  </si>
+  <si>
+    <t>Chr18_13070333_13297873</t>
+  </si>
+  <si>
+    <t>Rsquares</t>
+  </si>
+  <si>
+    <t>GenoName</t>
+  </si>
+  <si>
+    <t>D2.ND.0</t>
+  </si>
+  <si>
+    <t>D1.N1.2</t>
+  </si>
+  <si>
+    <t>D2.N1.2</t>
+  </si>
+  <si>
+    <t>D2.N2.1</t>
+  </si>
+  <si>
+    <t>D1.N1.1 / D1.N1.2</t>
+  </si>
+  <si>
+    <t>Chr01_27147399_27908896</t>
+  </si>
+  <si>
+    <t>Chr01_29345990_36756946</t>
+  </si>
+  <si>
+    <t>S1S6</t>
+  </si>
+  <si>
+    <t>S2S3 / S2S4 / S2S5 / S2S6</t>
+  </si>
+  <si>
+    <t>S1S3 / S1S4 / S1S5 / S1S6</t>
+  </si>
+  <si>
+    <t>S2S5</t>
+  </si>
+  <si>
+    <t>S1S4</t>
+  </si>
+  <si>
+    <t>S3S6 / S5S6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1228,8 +1202,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1546,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8297DAF-26F7-D747-8F91-9C869A778B87}">
   <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G107" sqref="G107"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3135,8 +3110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6BFE61-05FE-3A4A-A3BE-24F5A469B700}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4332,8 +4307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D0E22D-56EA-714C-B12F-8D1249E9E279}">
   <dimension ref="A1:D322"/>
   <sheetViews>
-    <sheetView topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="H311" sqref="H311"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78:D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8861,126 +8836,127 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>359</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>362</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>227</v>
       </c>
       <c r="D2">
-        <v>3.9360766384499501</v>
+        <v>13.237558534302501</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>363</v>
       </c>
       <c r="C3" t="s">
         <v>354</v>
       </c>
       <c r="D3">
-        <v>7.9382414158903902</v>
+        <v>5.2225194514985898</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>364</v>
       </c>
       <c r="C4" t="s">
         <v>355</v>
       </c>
       <c r="D4">
-        <v>5.33659370766643</v>
+        <v>14.3018505539498</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>307</v>
+        <v>360</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>303</v>
       </c>
       <c r="D5">
-        <v>5.0930739622079999</v>
+        <v>4.5816281847976397</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>310</v>
+        <v>360</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>356</v>
       </c>
       <c r="D6">
-        <v>4.6939965159884496</v>
+        <v>7.0591532769490897</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>360</v>
       </c>
       <c r="C7" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="D7">
-        <v>5.6247094129593496</v>
+        <v>6.0953087978788396</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>361</v>
       </c>
       <c r="C8" t="s">
         <v>357</v>
       </c>
       <c r="D8">
-        <v>5.1129467054842204</v>
+        <v>3.6969606018777701</v>
       </c>
     </row>
   </sheetData>
@@ -8990,597 +8966,129 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D500A3F-65B2-7340-B3F2-5DFFAA8D13E6}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
+      <c r="D1" s="1" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>368</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="D2">
-        <v>4.59174899861185</v>
+        <v>13.2375585343026</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>367</v>
       </c>
       <c r="C3" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="D3">
-        <v>6.11887347416965</v>
+        <v>5.5095463550469699</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>367</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>176</v>
       </c>
       <c r="D4">
-        <v>7.4658680568087803</v>
+        <v>5.1123589931524602</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>369</v>
       </c>
       <c r="C5" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
       <c r="D5">
-        <v>4.2802842822900198</v>
+        <v>15.242407991255201</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>372</v>
       </c>
       <c r="C6" t="s">
-        <v>359</v>
+        <v>135</v>
       </c>
       <c r="D6">
-        <v>5.6303425574876398</v>
+        <v>7.47366833090308</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>370</v>
       </c>
       <c r="C7" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D7">
-        <v>5.8353793376496297</v>
+        <v>7.0591532769490897</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>371</v>
       </c>
       <c r="C8" t="s">
-        <v>361</v>
+        <v>212</v>
       </c>
       <c r="D8">
-        <v>6.6597336171513497</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" t="s">
-        <v>173</v>
-      </c>
-      <c r="D9">
-        <v>7.1427849840325104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>156</v>
-      </c>
-      <c r="B10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" t="s">
-        <v>362</v>
-      </c>
-      <c r="D10">
-        <v>4.5031042021363099</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>156</v>
-      </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" t="s">
-        <v>361</v>
-      </c>
-      <c r="D11">
-        <v>6.3894924799632404</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84513E66-1701-CD46-91A5-B58572DFE97F}">
-  <dimension ref="A1:D29"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="46.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>363</v>
-      </c>
-      <c r="D2">
-        <v>2.8634657744688798</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>364</v>
-      </c>
-      <c r="D3">
-        <v>2.8549695098647598</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B4" t="s">
-        <v>365</v>
-      </c>
-      <c r="C4" t="s">
-        <v>363</v>
-      </c>
-      <c r="D4">
-        <v>3.0210306951912398</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" t="s">
-        <v>365</v>
-      </c>
-      <c r="C5" t="s">
-        <v>364</v>
-      </c>
-      <c r="D5">
-        <v>2.86501855573096</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>366</v>
-      </c>
-      <c r="D6">
-        <v>4.4501302208014701</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>155</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>364</v>
-      </c>
-      <c r="D7">
-        <v>2.94329816575245</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>155</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>367</v>
-      </c>
-      <c r="D8">
-        <v>6.1929638203534498</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>155</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>368</v>
-      </c>
-      <c r="D9">
-        <v>7.98251080595253</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>369</v>
-      </c>
-      <c r="D10">
-        <v>7.4430446928863496</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>155</v>
-      </c>
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>370</v>
-      </c>
-      <c r="D11">
-        <v>6.9263751340082003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B12" t="s">
-        <v>138</v>
-      </c>
-      <c r="C12" t="s">
-        <v>368</v>
-      </c>
-      <c r="D12">
-        <v>7.39006809102783</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>155</v>
-      </c>
-      <c r="B13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C13" t="s">
-        <v>371</v>
-      </c>
-      <c r="D13">
-        <v>5.1288516786328904</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>155</v>
-      </c>
-      <c r="B14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C14" t="s">
-        <v>372</v>
-      </c>
-      <c r="D14">
-        <v>8.1573365232888602</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>155</v>
-      </c>
-      <c r="B15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" t="s">
-        <v>366</v>
-      </c>
-      <c r="D15">
-        <v>3.5971689355505601</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>155</v>
-      </c>
-      <c r="B16" t="s">
-        <v>273</v>
-      </c>
-      <c r="C16" t="s">
-        <v>366</v>
-      </c>
-      <c r="D16">
-        <v>4.0671413383251496</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>155</v>
-      </c>
-      <c r="B17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" t="s">
-        <v>363</v>
-      </c>
-      <c r="D17">
-        <v>7.6223388089608202</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>156</v>
-      </c>
-      <c r="B18" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" t="s">
-        <v>373</v>
-      </c>
-      <c r="D18">
-        <v>3.48058836522336</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>156</v>
-      </c>
-      <c r="B19" t="s">
-        <v>95</v>
-      </c>
-      <c r="C19" t="s">
-        <v>374</v>
-      </c>
-      <c r="D19">
-        <v>6.3416788901781302</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>156</v>
-      </c>
-      <c r="B20" t="s">
-        <v>307</v>
-      </c>
-      <c r="C20" t="s">
-        <v>375</v>
-      </c>
-      <c r="D20">
-        <v>7.4669599742945101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>156</v>
-      </c>
-      <c r="B21" t="s">
-        <v>307</v>
-      </c>
-      <c r="C21" t="s">
-        <v>376</v>
-      </c>
-      <c r="D21">
-        <v>5.8251816638368901</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>156</v>
-      </c>
-      <c r="B22" t="s">
-        <v>307</v>
-      </c>
-      <c r="C22" t="s">
-        <v>377</v>
-      </c>
-      <c r="D22">
-        <v>10.0110353002763</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B23" t="s">
-        <v>307</v>
-      </c>
-      <c r="C23" t="s">
-        <v>378</v>
-      </c>
-      <c r="D23">
-        <v>19.309049111620698</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>156</v>
-      </c>
-      <c r="B24" t="s">
-        <v>105</v>
-      </c>
-      <c r="C24" t="s">
-        <v>379</v>
-      </c>
-      <c r="D24">
-        <v>9.0018871540275693</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>156</v>
-      </c>
-      <c r="B25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" t="s">
-        <v>380</v>
-      </c>
-      <c r="D25">
-        <v>9.4297473665630207</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>156</v>
-      </c>
-      <c r="B26" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" t="s">
-        <v>381</v>
-      </c>
-      <c r="D26">
-        <v>8.0494022449165001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>156</v>
-      </c>
-      <c r="B27" t="s">
-        <v>110</v>
-      </c>
-      <c r="C27" t="s">
-        <v>376</v>
-      </c>
-      <c r="D27">
-        <v>4.3213116426989799</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>156</v>
-      </c>
-      <c r="B28" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" t="s">
-        <v>382</v>
-      </c>
-      <c r="D28">
-        <v>3.3372359566877701</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>156</v>
-      </c>
-      <c r="B29" t="s">
-        <v>113</v>
-      </c>
-      <c r="C29" t="s">
-        <v>383</v>
-      </c>
-      <c r="D29">
-        <v>7.5221981197709802</v>
+        <v>4.4174356798226997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>